<commit_message>
Enhancements 56 & 57
</commit_message>
<xml_diff>
--- a/app/templates/report/contratos.xlsx
+++ b/app/templates/report/contratos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07dae84afc6a2e79/Development/projects/ciber/cotown/back/app/templates/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{606EB427-8D04-4765-819B-198FFB7C46F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A6A356-7455-4E05-BAE9-B65347EB5419}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325DFEFA-992D-4073-8A0E-A0CE41C031B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Contratos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contratos!$A$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contratos!$A$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -185,7 +185,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -275,14 +275,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -320,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -426,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -568,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -576,7 +572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,20 +581,20 @@
     <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="41.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="24.85546875" style="1"/>
+    <col min="4" max="5" width="48.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="41.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="24.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -609,41 +605,43 @@
         <v>7</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:J2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>